<commit_message>
Avances en el diseno
</commit_message>
<xml_diff>
--- a/Ex4/TP3E4_PROJ.xlsx
+++ b/Ex4/TP3E4_PROJ.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ohvic\Documents\ITBA\TP03\Ex4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A9F1E2D1-FC54-4C26-AB10-9BFA7377C539}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEFA8CBF-2E1D-456D-8495-34C744A45266}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23775" yWindow="4500" windowWidth="28800" windowHeight="11325" activeTab="2" xr2:uid="{0C1CF8BA-2CF4-460A-BC3B-92718A0B8CD2}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{0C1CF8BA-2CF4-460A-BC3B-92718A0B8CD2}"/>
   </bookViews>
   <sheets>
     <sheet name="TRABAJO" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="64">
   <si>
     <t>TASK</t>
   </si>
@@ -224,6 +224,9 @@
   </si>
   <si>
     <t>mV/kPa</t>
+  </si>
+  <si>
+    <t>LM833 con +VCC=15 y -VCC=0?</t>
   </si>
 </sst>
 </file>
@@ -583,18 +586,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68A02374-079C-46DF-BD9A-C943DF6F482D}">
   <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="30.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="44" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="42.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="42.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -608,7 +611,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -616,7 +619,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -624,7 +627,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -632,7 +635,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -640,7 +643,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -648,39 +651,51 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>2</v>
       </c>
       <c r="B7" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C7">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>2</v>
       </c>
       <c r="B8" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C8">
+        <v>1522</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>2</v>
       </c>
       <c r="B9" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>2</v>
       </c>
       <c r="B10" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -688,7 +703,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -696,7 +711,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -704,7 +719,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>11</v>
       </c>
@@ -712,7 +727,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>11</v>
       </c>
@@ -720,7 +735,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>25</v>
       </c>
@@ -728,7 +743,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>25</v>
       </c>
@@ -736,7 +751,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>25</v>
       </c>
@@ -747,7 +762,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>25</v>
       </c>
@@ -755,7 +770,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>26</v>
       </c>
@@ -763,7 +778,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>26</v>
       </c>
@@ -771,7 +786,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>26</v>
       </c>
@@ -779,7 +794,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>26</v>
       </c>
@@ -787,7 +802,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>30</v>
       </c>
@@ -795,7 +810,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>30</v>
       </c>
@@ -803,7 +818,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>30</v>
       </c>
@@ -831,13 +846,13 @@
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="36.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="36.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -845,7 +860,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>36</v>
       </c>
@@ -853,17 +868,17 @@
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>38</v>
       </c>
@@ -871,22 +886,22 @@
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>43</v>
       </c>
@@ -894,17 +909,17 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>45</v>
       </c>
@@ -918,16 +933,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C609BFC3-41F9-46DD-9E11-68074C57E8AC}">
   <dimension ref="A1:E31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>46</v>
       </c>
@@ -944,7 +959,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>55</v>
       </c>
@@ -961,7 +976,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>56</v>
       </c>
@@ -978,7 +993,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>58</v>
       </c>
@@ -995,7 +1010,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>54</v>
       </c>
@@ -1012,7 +1027,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>60</v>
       </c>
@@ -1029,7 +1044,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>61</v>
       </c>
@@ -1046,122 +1061,122 @@
         <v>62</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
     </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
     </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
     </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
     </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
     </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
     </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
     </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
     </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
     </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
     </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
     </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
       <c r="D31" s="1"/>

</xml_diff>

<commit_message>
Muchos cambios y correcciones. Informe Listo
</commit_message>
<xml_diff>
--- a/Ex4/TP3E4_PROJ.xlsx
+++ b/Ex4/TP3E4_PROJ.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ohvic\Documents\ITBA\TP03\Ex4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{493690B9-FAA1-4D63-8718-BDE9200BD0F7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E5ED6D9-D03E-45C1-A5D7-B682A9E0428D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" activeTab="4" xr2:uid="{0C1CF8BA-2CF4-460A-BC3B-92718A0B8CD2}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{0C1CF8BA-2CF4-460A-BC3B-92718A0B8CD2}"/>
   </bookViews>
   <sheets>
     <sheet name="TRABAJO" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="75">
   <si>
     <t>TASK</t>
   </si>
@@ -231,28 +231,37 @@
     <t>LM833 con +VCC=15 y -VCC=-15</t>
   </si>
   <si>
-    <t>Vin / V</t>
-  </si>
-  <si>
-    <t>Vout / V</t>
-  </si>
-  <si>
     <t>VoutDM / V</t>
   </si>
   <si>
-    <t>VoutCM / V</t>
-  </si>
-  <si>
     <t>ADM</t>
   </si>
   <si>
-    <t>ACM</t>
-  </si>
-  <si>
-    <t>CMRR / dB</t>
-  </si>
-  <si>
-    <t>h(H2O) / m</t>
+    <t>VinDM / V</t>
+  </si>
+  <si>
+    <t>DVdm</t>
+  </si>
+  <si>
+    <t>Adm2</t>
+  </si>
+  <si>
+    <t>Cano/cm</t>
+  </si>
+  <si>
+    <t>Tubo/cm</t>
+  </si>
+  <si>
+    <t>D Altura/m</t>
+  </si>
+  <si>
+    <t>Vout/V</t>
+  </si>
+  <si>
+    <t>No se puede medir V cm por sobre el piso de ruido</t>
+  </si>
+  <si>
+    <t>sin off</t>
   </si>
 </sst>
 </file>
@@ -262,7 +271,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -270,18 +279,67 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor theme="4" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </left>
       <right/>
       <top/>
       <bottom/>
@@ -291,7 +349,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -300,11 +358,62 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="18">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="0.000"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="0.000"/>
     </dxf>
@@ -312,16 +421,272 @@
       <numFmt numFmtId="164" formatCode="0.000"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="164" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
       <numFmt numFmtId="0" formatCode="General"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom/>
+      </border>
     </dxf>
     <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
       <numFmt numFmtId="164" formatCode="0.000"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="0.000"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="0.000"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="0.000"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <right style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </right>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -337,20 +702,20 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{ABEB69B3-03F5-4CC6-9D74-EBA0C0EDBF06}" name="Table1" displayName="Table1" ref="A1:F11" totalsRowShown="0">
-  <autoFilter ref="A1:F11" xr:uid="{237DA04C-0F6E-455A-B001-C36C353F70DD}"/>
-  <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{CFBE27F0-DB98-4A1D-82BA-BCE3FBB540B8}" name="Vin / V" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{92BE880B-7A14-4B08-B22B-AAB703BC1B56}" name="VoutDM / V"/>
-    <tableColumn id="3" xr3:uid="{732CFCE2-754D-4A36-A545-95B1B39CB837}" name="VoutCM / V"/>
-    <tableColumn id="4" xr3:uid="{667D529A-CC4C-4464-8E62-1C2FE60B49F9}" name="ADM" dataDxfId="3">
-      <calculatedColumnFormula>Table1[[#This Row],[VoutDM / V]]/Table1[[#This Row],[Vin / V]]</calculatedColumnFormula>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{E3062D9F-1548-43DB-8C5A-B1BB0BB64DFD}" name="Table5" displayName="Table5" ref="A1:E12" totalsRowCount="1" headerRowDxfId="17" dataDxfId="16" tableBorderDxfId="15">
+  <autoFilter ref="A1:E11" xr:uid="{0ACE26C8-9229-4BC8-96E8-D82653DE00E2}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{34950A47-241D-430F-9516-970B9DB2B0DE}" name="VinDM / V" dataDxfId="14" totalsRowDxfId="13"/>
+    <tableColumn id="2" xr3:uid="{4EFC090F-DD67-4C77-A02E-A8A46C91CF26}" name="VoutDM / V" dataDxfId="12" totalsRowDxfId="11"/>
+    <tableColumn id="5" xr3:uid="{E36A6CB1-5584-4526-996F-7C6753F4BD83}" name="ADM" dataDxfId="10" totalsRowDxfId="9">
+      <calculatedColumnFormula>Table5[[#This Row],[VoutDM / V]]/Table5[[#This Row],[VinDM / V]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{DF87CFA5-D68C-4C94-8350-45CD7119CC42}" name="ACM" dataDxfId="2">
-      <calculatedColumnFormula>Table1[[#This Row],[VoutCM / V]]/Table1[[#This Row],[Vin / V]]</calculatedColumnFormula>
+    <tableColumn id="8" xr3:uid="{AD0A60E3-7F24-434E-A22A-2919D57D07AE}" name="DVdm" dataDxfId="0" totalsRowDxfId="1">
+      <calculatedColumnFormula>Table5[[#This Row],[VoutDM / V]]-$B$11</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{45E51751-24CC-44E4-A6E3-7C6B9886F9DC}" name="CMRR / dB" dataDxfId="4">
-      <calculatedColumnFormula>10*LOG10(Table1[[#This Row],[ADM]]/Table1[[#This Row],[ACM]])</calculatedColumnFormula>
+    <tableColumn id="10" xr3:uid="{85E94E72-3EEF-4F3B-BB90-1613BCE80B26}" name="Adm2" totalsRowFunction="custom" dataDxfId="8" totalsRowDxfId="7">
+      <calculatedColumnFormula>Table5[[#This Row],[DVdm]]/Table5[[#This Row],[VinDM / V]]</calculatedColumnFormula>
+      <totalsRowFormula>AVERAGE(E2:E10)</totalsRowFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -358,11 +723,18 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2EEF8498-0D2F-426F-854C-0FF51A23A0DB}" name="Table13" displayName="Table13" ref="A1:B12" totalsRowShown="0">
-  <autoFilter ref="A1:B12" xr:uid="{237DA04C-0F6E-455A-B001-C36C353F70DD}"/>
-  <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{595BFDD5-62D0-4F03-89AC-9D3206F26824}" name="h(H2O) / m" dataDxfId="0"/>
-    <tableColumn id="7" xr3:uid="{B13209F0-8417-491E-9C54-BCFF1756BC87}" name="Vout / V" dataDxfId="1"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2EEF8498-0D2F-426F-854C-0FF51A23A0DB}" name="Table13" displayName="Table13" ref="A1:E12" totalsRowShown="0">
+  <autoFilter ref="A1:E12" xr:uid="{237DA04C-0F6E-455A-B001-C36C353F70DD}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{595BFDD5-62D0-4F03-89AC-9D3206F26824}" name="Cano/cm" dataDxfId="6"/>
+    <tableColumn id="7" xr3:uid="{B13209F0-8417-491E-9C54-BCFF1756BC87}" name="Tubo/cm" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{2537676D-179C-4DB9-9D95-C1E2533EF302}" name="D Altura/m" dataDxfId="4">
+      <calculatedColumnFormula>(Table13[[#This Row],[Cano/cm]]-Table13[[#This Row],[Tubo/cm]])/100</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="3" xr3:uid="{2197A237-9456-47C8-93A9-546E89264176}" name="Vout/V" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{5DB7072F-2153-4787-A01F-7A17CAA59B74}" name="sin off" dataDxfId="2">
+      <calculatedColumnFormula>Table13[[#This Row],[Vout/V]]-$D$2</calculatedColumnFormula>
+    </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -667,18 +1039,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68A02374-079C-46DF-BD9A-C943DF6F482D}">
   <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="30.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="44" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="42.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="42.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -692,7 +1064,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -703,7 +1075,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -714,7 +1086,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -725,7 +1097,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -736,7 +1108,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -747,7 +1119,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>2</v>
       </c>
@@ -761,7 +1133,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>2</v>
       </c>
@@ -775,7 +1147,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>2</v>
       </c>
@@ -789,7 +1161,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>2</v>
       </c>
@@ -803,7 +1175,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -814,7 +1186,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -825,7 +1197,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -836,7 +1208,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>11</v>
       </c>
@@ -847,7 +1219,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>11</v>
       </c>
@@ -858,7 +1230,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>25</v>
       </c>
@@ -866,7 +1238,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>25</v>
       </c>
@@ -874,7 +1246,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>25</v>
       </c>
@@ -885,7 +1257,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>25</v>
       </c>
@@ -893,7 +1265,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>26</v>
       </c>
@@ -904,7 +1276,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>26</v>
       </c>
@@ -915,7 +1287,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>26</v>
       </c>
@@ -926,7 +1298,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>26</v>
       </c>
@@ -937,7 +1309,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>30</v>
       </c>
@@ -948,7 +1320,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>30</v>
       </c>
@@ -959,7 +1331,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>30</v>
       </c>
@@ -990,13 +1362,13 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="36.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="36.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1004,7 +1376,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>36</v>
       </c>
@@ -1012,17 +1384,17 @@
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>38</v>
       </c>
@@ -1030,22 +1402,22 @@
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>43</v>
       </c>
@@ -1053,17 +1425,17 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>45</v>
       </c>
@@ -1081,12 +1453,12 @@
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>46</v>
       </c>
@@ -1103,7 +1475,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>55</v>
       </c>
@@ -1120,7 +1492,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>56</v>
       </c>
@@ -1137,7 +1509,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>58</v>
       </c>
@@ -1154,7 +1526,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>54</v>
       </c>
@@ -1171,7 +1543,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>60</v>
       </c>
@@ -1188,7 +1560,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>61</v>
       </c>
@@ -1205,122 +1577,122 @@
         <v>62</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
     </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
     </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
     </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
     </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
     </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
     </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
     </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
     </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
     </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
     </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
     </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
       <c r="D31" s="1"/>
@@ -1332,208 +1704,246 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62DEECF7-215A-4866-A36A-F0CED8483611}">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="3"/>
-    <col min="2" max="2" width="13.5703125" customWidth="1"/>
-    <col min="3" max="3" width="13.42578125" customWidth="1"/>
-    <col min="6" max="6" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.6640625" customWidth="1"/>
+    <col min="2" max="2" width="13.33203125" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B1" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="B1" t="s">
-        <v>66</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="C1" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D1" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="E1" t="s">
-        <v>69</v>
-      </c>
-      <c r="F1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="3">
-        <v>0.1</v>
-      </c>
-      <c r="D2">
-        <f>Table1[[#This Row],[VoutDM / V]]/Table1[[#This Row],[Vin / V]]</f>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" s="5">
+        <v>0.06</v>
+      </c>
+      <c r="B2" s="9">
+        <v>7.9130000000000003</v>
+      </c>
+      <c r="C2" s="6">
+        <f>Table5[[#This Row],[VoutDM / V]]/Table5[[#This Row],[VinDM / V]]</f>
+        <v>131.88333333333335</v>
+      </c>
+      <c r="D2" s="14">
+        <f>Table5[[#This Row],[VoutDM / V]]-$B$11</f>
+        <v>7.6989999999999998</v>
+      </c>
+      <c r="E2" s="12">
+        <f>Table5[[#This Row],[DVdm]]/Table5[[#This Row],[VinDM / V]]</f>
+        <v>128.31666666666666</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" s="7">
+        <v>0.05</v>
+      </c>
+      <c r="B3" s="7">
+        <v>6.6230000000000002</v>
+      </c>
+      <c r="C3" s="8">
+        <f>Table5[[#This Row],[VoutDM / V]]/Table5[[#This Row],[VinDM / V]]</f>
+        <v>132.46</v>
+      </c>
+      <c r="D3" s="14">
+        <f>Table5[[#This Row],[VoutDM / V]]-$B$11</f>
+        <v>6.4089999999999998</v>
+      </c>
+      <c r="E3" s="12">
+        <f>Table5[[#This Row],[DVdm]]/Table5[[#This Row],[VinDM / V]]</f>
+        <v>128.17999999999998</v>
+      </c>
+      <c r="H3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" s="5">
+        <v>0.04</v>
+      </c>
+      <c r="B4" s="7">
+        <v>5.3410000000000002</v>
+      </c>
+      <c r="C4" s="6">
+        <f>Table5[[#This Row],[VoutDM / V]]/Table5[[#This Row],[VinDM / V]]</f>
+        <v>133.52500000000001</v>
+      </c>
+      <c r="D4" s="14">
+        <f>Table5[[#This Row],[VoutDM / V]]-$B$11</f>
+        <v>5.1269999999999998</v>
+      </c>
+      <c r="E4" s="12">
+        <f>Table5[[#This Row],[DVdm]]/Table5[[#This Row],[VinDM / V]]</f>
+        <v>128.17499999999998</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" s="7">
+        <v>0.03</v>
+      </c>
+      <c r="B5" s="7">
+        <v>4.0590000000000002</v>
+      </c>
+      <c r="C5" s="8">
+        <f>Table5[[#This Row],[VoutDM / V]]/Table5[[#This Row],[VinDM / V]]</f>
+        <v>135.30000000000001</v>
+      </c>
+      <c r="D5" s="14">
+        <f>Table5[[#This Row],[VoutDM / V]]-$B$11</f>
+        <v>3.8450000000000002</v>
+      </c>
+      <c r="E5" s="12">
+        <f>Table5[[#This Row],[DVdm]]/Table5[[#This Row],[VinDM / V]]</f>
+        <v>128.16666666666669</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" s="5">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="B6" s="7">
+        <v>3.4049999999999998</v>
+      </c>
+      <c r="C6" s="6">
+        <f>Table5[[#This Row],[VoutDM / V]]/Table5[[#This Row],[VinDM / V]]</f>
+        <v>136.19999999999999</v>
+      </c>
+      <c r="D6" s="14">
+        <f>Table5[[#This Row],[VoutDM / V]]-$B$11</f>
+        <v>3.1909999999999998</v>
+      </c>
+      <c r="E6" s="12">
+        <f>Table5[[#This Row],[DVdm]]/Table5[[#This Row],[VinDM / V]]</f>
+        <v>127.63999999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" s="7">
+        <v>0.02</v>
+      </c>
+      <c r="B7" s="7">
+        <v>2.7730000000000001</v>
+      </c>
+      <c r="C7" s="10">
+        <f>Table5[[#This Row],[VoutDM / V]]/Table5[[#This Row],[VinDM / V]]</f>
+        <v>138.65</v>
+      </c>
+      <c r="D7" s="14">
+        <f>Table5[[#This Row],[VoutDM / V]]-$B$11</f>
+        <v>2.5590000000000002</v>
+      </c>
+      <c r="E7" s="12">
+        <f>Table5[[#This Row],[DVdm]]/Table5[[#This Row],[VinDM / V]]</f>
+        <v>127.95</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" s="7">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="B8" s="7">
+        <v>2.1240000000000001</v>
+      </c>
+      <c r="C8" s="10">
+        <f>Table5[[#This Row],[VoutDM / V]]/Table5[[#This Row],[VinDM / V]]</f>
+        <v>141.60000000000002</v>
+      </c>
+      <c r="D8" s="14">
+        <f>Table5[[#This Row],[VoutDM / V]]-$B$11</f>
+        <v>1.9100000000000001</v>
+      </c>
+      <c r="E8" s="12">
+        <f>Table5[[#This Row],[DVdm]]/Table5[[#This Row],[VinDM / V]]</f>
+        <v>127.33333333333334</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" s="7">
+        <v>0.01</v>
+      </c>
+      <c r="B9" s="7">
+        <v>1.496</v>
+      </c>
+      <c r="C9" s="10">
+        <f>Table5[[#This Row],[VoutDM / V]]/Table5[[#This Row],[VinDM / V]]</f>
+        <v>149.6</v>
+      </c>
+      <c r="D9" s="14">
+        <f>Table5[[#This Row],[VoutDM / V]]-$B$11</f>
+        <v>1.282</v>
+      </c>
+      <c r="E9" s="12">
+        <f>Table5[[#This Row],[DVdm]]/Table5[[#This Row],[VinDM / V]]</f>
+        <v>128.19999999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10" s="7">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="B10" s="7">
+        <v>0.84299999999999997</v>
+      </c>
+      <c r="C10" s="10">
+        <f>Table5[[#This Row],[VoutDM / V]]/Table5[[#This Row],[VinDM / V]]</f>
+        <v>168.6</v>
+      </c>
+      <c r="D10" s="14">
+        <f>Table5[[#This Row],[VoutDM / V]]-$B$11</f>
+        <v>0.629</v>
+      </c>
+      <c r="E10" s="12">
+        <f>Table5[[#This Row],[DVdm]]/Table5[[#This Row],[VinDM / V]]</f>
+        <v>125.8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11" s="7">
         <v>0</v>
       </c>
-      <c r="E2">
-        <f>Table1[[#This Row],[VoutCM / V]]/Table1[[#This Row],[Vin / V]]</f>
+      <c r="B11" s="7">
+        <v>0.214</v>
+      </c>
+      <c r="C11" s="10" t="e">
+        <f>Table5[[#This Row],[VoutDM / V]]/Table5[[#This Row],[VinDM / V]]</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D11" s="14">
+        <f>Table5[[#This Row],[VoutDM / V]]-$B$11</f>
         <v>0</v>
       </c>
-      <c r="F2" t="e">
-        <f>10*LOG10(Table1[[#This Row],[ADM]]/Table1[[#This Row],[ACM]])</f>
+      <c r="E11" s="12" t="e">
+        <f>Table5[[#This Row],[DVdm]]/Table5[[#This Row],[VinDM / V]]</f>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="3">
-        <v>0.2</v>
-      </c>
-      <c r="D3">
-        <f>Table1[[#This Row],[VoutDM / V]]/Table1[[#This Row],[Vin / V]]</f>
-        <v>0</v>
-      </c>
-      <c r="E3">
-        <f>Table1[[#This Row],[VoutCM / V]]/Table1[[#This Row],[Vin / V]]</f>
-        <v>0</v>
-      </c>
-      <c r="F3" t="e">
-        <f>10*LOG10(Table1[[#This Row],[ADM]]/Table1[[#This Row],[ACM]])</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="3">
-        <v>0.3</v>
-      </c>
-      <c r="D4">
-        <f>Table1[[#This Row],[VoutDM / V]]/Table1[[#This Row],[Vin / V]]</f>
-        <v>0</v>
-      </c>
-      <c r="E4">
-        <f>Table1[[#This Row],[VoutCM / V]]/Table1[[#This Row],[Vin / V]]</f>
-        <v>0</v>
-      </c>
-      <c r="F4" t="e">
-        <f>10*LOG10(Table1[[#This Row],[ADM]]/Table1[[#This Row],[ACM]])</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="3">
-        <v>0.4</v>
-      </c>
-      <c r="D5">
-        <f>Table1[[#This Row],[VoutDM / V]]/Table1[[#This Row],[Vin / V]]</f>
-        <v>0</v>
-      </c>
-      <c r="E5">
-        <f>Table1[[#This Row],[VoutCM / V]]/Table1[[#This Row],[Vin / V]]</f>
-        <v>0</v>
-      </c>
-      <c r="F5" t="e">
-        <f>10*LOG10(Table1[[#This Row],[ADM]]/Table1[[#This Row],[ACM]])</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="D6">
-        <f>Table1[[#This Row],[VoutDM / V]]/Table1[[#This Row],[Vin / V]]</f>
-        <v>0</v>
-      </c>
-      <c r="E6">
-        <f>Table1[[#This Row],[VoutCM / V]]/Table1[[#This Row],[Vin / V]]</f>
-        <v>0</v>
-      </c>
-      <c r="F6" t="e">
-        <f>10*LOG10(Table1[[#This Row],[ADM]]/Table1[[#This Row],[ACM]])</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="3">
-        <v>0.6</v>
-      </c>
-      <c r="D7">
-        <f>Table1[[#This Row],[VoutDM / V]]/Table1[[#This Row],[Vin / V]]</f>
-        <v>0</v>
-      </c>
-      <c r="E7">
-        <f>Table1[[#This Row],[VoutCM / V]]/Table1[[#This Row],[Vin / V]]</f>
-        <v>0</v>
-      </c>
-      <c r="F7" t="e">
-        <f>10*LOG10(Table1[[#This Row],[ADM]]/Table1[[#This Row],[ACM]])</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="3">
-        <v>0.7</v>
-      </c>
-      <c r="D8">
-        <f>Table1[[#This Row],[VoutDM / V]]/Table1[[#This Row],[Vin / V]]</f>
-        <v>0</v>
-      </c>
-      <c r="E8">
-        <f>Table1[[#This Row],[VoutCM / V]]/Table1[[#This Row],[Vin / V]]</f>
-        <v>0</v>
-      </c>
-      <c r="F8" t="e">
-        <f>10*LOG10(Table1[[#This Row],[ADM]]/Table1[[#This Row],[ACM]])</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="3">
-        <v>0.8</v>
-      </c>
-      <c r="D9">
-        <f>Table1[[#This Row],[VoutDM / V]]/Table1[[#This Row],[Vin / V]]</f>
-        <v>0</v>
-      </c>
-      <c r="E9">
-        <f>Table1[[#This Row],[VoutCM / V]]/Table1[[#This Row],[Vin / V]]</f>
-        <v>0</v>
-      </c>
-      <c r="F9" t="e">
-        <f>10*LOG10(Table1[[#This Row],[ADM]]/Table1[[#This Row],[ACM]])</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="3">
-        <v>0.9</v>
-      </c>
-      <c r="D10">
-        <f>Table1[[#This Row],[VoutDM / V]]/Table1[[#This Row],[Vin / V]]</f>
-        <v>0</v>
-      </c>
-      <c r="E10">
-        <f>Table1[[#This Row],[VoutCM / V]]/Table1[[#This Row],[Vin / V]]</f>
-        <v>0</v>
-      </c>
-      <c r="F10" t="e">
-        <f>10*LOG10(Table1[[#This Row],[ADM]]/Table1[[#This Row],[ACM]])</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="3">
-        <v>1</v>
-      </c>
-      <c r="D11">
-        <f>Table1[[#This Row],[VoutDM / V]]/Table1[[#This Row],[Vin / V]]</f>
-        <v>0</v>
-      </c>
-      <c r="E11">
-        <f>Table1[[#This Row],[VoutCM / V]]/Table1[[#This Row],[Vin / V]]</f>
-        <v>0</v>
-      </c>
-      <c r="F11" t="e">
-        <f>10*LOG10(Table1[[#This Row],[ADM]]/Table1[[#This Row],[ACM]])</f>
-        <v>#DIV/0!</v>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12" s="7"/>
+      <c r="B12" s="7"/>
+      <c r="C12" s="10"/>
+      <c r="D12" s="14"/>
+      <c r="E12" s="15">
+        <f>AVERAGE(E2:E10)</f>
+        <v>127.7512962962963</v>
       </c>
     </row>
   </sheetData>
@@ -1546,91 +1956,244 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3FE6AB62-93B8-4E06-ADD7-0AA91AAE6EFA}">
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.6640625" style="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5546875" style="16" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="16" t="s">
+        <v>69</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="C1" t="s">
         <v>71</v>
       </c>
-      <c r="B1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="3">
+      <c r="D1" t="s">
+        <v>72</v>
+      </c>
+      <c r="E1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="16">
         <v>0</v>
       </c>
-      <c r="B2" s="3"/>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="3">
+      <c r="B2" s="16">
+        <v>0</v>
+      </c>
+      <c r="C2" s="3">
+        <f>(Table13[[#This Row],[Cano/cm]]-Table13[[#This Row],[Tubo/cm]])/100</f>
+        <v>0</v>
+      </c>
+      <c r="D2" s="3">
+        <v>0.253</v>
+      </c>
+      <c r="E2" s="3">
+        <f>Table13[[#This Row],[Vout/V]]-$D$2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="16">
+        <v>18</v>
+      </c>
+      <c r="B3" s="16">
+        <v>8</v>
+      </c>
+      <c r="C3" s="3">
+        <f>(Table13[[#This Row],[Cano/cm]]-Table13[[#This Row],[Tubo/cm]])/100</f>
         <v>0.1</v>
       </c>
-      <c r="B3" s="3"/>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="3">
-        <v>0.2</v>
-      </c>
-      <c r="B4" s="3"/>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="3">
-        <v>0.3</v>
-      </c>
-      <c r="B5" s="3"/>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="3">
+      <c r="D3" s="3">
+        <v>0.64400000000000002</v>
+      </c>
+      <c r="E3" s="3">
+        <f>Table13[[#This Row],[Vout/V]]-$D$2</f>
+        <v>0.39100000000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="16">
+        <v>30</v>
+      </c>
+      <c r="B4" s="16">
+        <v>11</v>
+      </c>
+      <c r="C4" s="3">
+        <f>(Table13[[#This Row],[Cano/cm]]-Table13[[#This Row],[Tubo/cm]])/100</f>
+        <v>0.19</v>
+      </c>
+      <c r="D4" s="3">
+        <v>0.91500000000000004</v>
+      </c>
+      <c r="E4" s="3">
+        <f>Table13[[#This Row],[Vout/V]]-$D$2</f>
+        <v>0.66200000000000003</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="16">
+        <v>48</v>
+      </c>
+      <c r="B5" s="16">
+        <v>17</v>
+      </c>
+      <c r="C5" s="3">
+        <f>(Table13[[#This Row],[Cano/cm]]-Table13[[#This Row],[Tubo/cm]])/100</f>
+        <v>0.31</v>
+      </c>
+      <c r="D5" s="3">
+        <v>1.2769999999999999</v>
+      </c>
+      <c r="E5" s="3">
+        <f>Table13[[#This Row],[Vout/V]]-$D$2</f>
+        <v>1.024</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="16">
+        <v>60</v>
+      </c>
+      <c r="B6" s="16">
+        <v>20</v>
+      </c>
+      <c r="C6" s="3">
+        <f>(Table13[[#This Row],[Cano/cm]]-Table13[[#This Row],[Tubo/cm]])/100</f>
         <v>0.4</v>
       </c>
-      <c r="B6" s="3"/>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="B7" s="3"/>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="3">
-        <v>0.6</v>
-      </c>
-      <c r="B8" s="3"/>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="3">
-        <v>0.7</v>
-      </c>
-      <c r="B9" s="3"/>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="3">
-        <v>0.8</v>
-      </c>
-      <c r="B10" s="3"/>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="3">
-        <v>0.9</v>
-      </c>
-      <c r="B11" s="3"/>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="3">
-        <v>1</v>
-      </c>
-      <c r="B12" s="3"/>
+      <c r="D6" s="3">
+        <v>1.577</v>
+      </c>
+      <c r="E6" s="3">
+        <f>Table13[[#This Row],[Vout/V]]-$D$2</f>
+        <v>1.3239999999999998</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="16">
+        <v>80</v>
+      </c>
+      <c r="B7" s="16">
+        <v>25</v>
+      </c>
+      <c r="C7" s="3">
+        <f>(Table13[[#This Row],[Cano/cm]]-Table13[[#This Row],[Tubo/cm]])/100</f>
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="D7" s="3">
+        <v>2.044</v>
+      </c>
+      <c r="E7" s="3">
+        <f>Table13[[#This Row],[Vout/V]]-$D$2</f>
+        <v>1.7909999999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" s="16">
+        <v>96</v>
+      </c>
+      <c r="B8" s="16">
+        <v>29</v>
+      </c>
+      <c r="C8" s="3">
+        <f>(Table13[[#This Row],[Cano/cm]]-Table13[[#This Row],[Tubo/cm]])/100</f>
+        <v>0.67</v>
+      </c>
+      <c r="D8" s="3">
+        <v>2.4049999999999998</v>
+      </c>
+      <c r="E8" s="3">
+        <f>Table13[[#This Row],[Vout/V]]-$D$2</f>
+        <v>2.1519999999999997</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" s="16">
+        <v>105</v>
+      </c>
+      <c r="B9" s="16">
+        <v>32</v>
+      </c>
+      <c r="C9" s="3">
+        <f>(Table13[[#This Row],[Cano/cm]]-Table13[[#This Row],[Tubo/cm]])/100</f>
+        <v>0.73</v>
+      </c>
+      <c r="D9" s="3">
+        <v>2.649</v>
+      </c>
+      <c r="E9" s="3">
+        <f>Table13[[#This Row],[Vout/V]]-$D$2</f>
+        <v>2.3959999999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" s="16">
+        <v>121</v>
+      </c>
+      <c r="B10" s="16">
+        <v>35</v>
+      </c>
+      <c r="C10" s="3">
+        <f>(Table13[[#This Row],[Cano/cm]]-Table13[[#This Row],[Tubo/cm]])/100</f>
+        <v>0.86</v>
+      </c>
+      <c r="D10" s="3">
+        <v>2.9929999999999999</v>
+      </c>
+      <c r="E10" s="3">
+        <f>Table13[[#This Row],[Vout/V]]-$D$2</f>
+        <v>2.7399999999999998</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" s="16">
+        <v>135</v>
+      </c>
+      <c r="B11" s="16">
+        <v>39</v>
+      </c>
+      <c r="C11" s="3">
+        <f>(Table13[[#This Row],[Cano/cm]]-Table13[[#This Row],[Tubo/cm]])/100</f>
+        <v>0.96</v>
+      </c>
+      <c r="D11" s="3">
+        <v>3.3330000000000002</v>
+      </c>
+      <c r="E11" s="3">
+        <f>Table13[[#This Row],[Vout/V]]-$D$2</f>
+        <v>3.08</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" s="16">
+        <v>143</v>
+      </c>
+      <c r="B12" s="16">
+        <v>41</v>
+      </c>
+      <c r="C12" s="3">
+        <f>(Table13[[#This Row],[Cano/cm]]-Table13[[#This Row],[Tubo/cm]])/100</f>
+        <v>1.02</v>
+      </c>
+      <c r="D12" s="3">
+        <v>3.5390000000000001</v>
+      </c>
+      <c r="E12" s="3">
+        <f>Table13[[#This Row],[Vout/V]]-$D$2</f>
+        <v>3.286</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>